<commit_message>
Hot fix: Markery teď zase na mapě sedí
</commit_message>
<xml_diff>
--- a/schools_legacy.xlsx
+++ b/schools_legacy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/majdikleckerova/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/226e3371a49bebd4/Dokumenty/MFVS stuff/Erasmus-visual-streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE7656C-4A7B-C244-BAC7-EEEDDC33082B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{6CE7656C-4A7B-C244-BAC7-EEEDDC33082B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC5CC996-C55B-4401-AD24-ED09FAB5FA5F}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="500" windowWidth="29420" windowHeight="19060" xr2:uid="{EAAF1794-3029-8A44-8037-036BBE2083F3}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{EAAF1794-3029-8A44-8037-036BBE2083F3}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1281,6 +1281,293 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1321,293 +1608,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1622,17 +1622,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8ECA42F5-AD48-8346-87D1-83B77664CA2A}" name="Tabulka1" displayName="Tabulka1" ref="A1:H95" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:H95" xr:uid="{8ECA42F5-AD48-8346-87D1-83B77664CA2A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8ECA42F5-AD48-8346-87D1-83B77664CA2A}" name="Tabulka1" displayName="Tabulka1" ref="A1:H95" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H95" xr:uid="{8ECA42F5-AD48-8346-87D1-83B77664CA2A}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Zagreb"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F1C2FD06-28A1-D847-971D-93220E657CA3}" name="Katedra" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{CDA11F7E-DE5E-5442-8805-D34B212F75F4}" name="Univerzita" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{27C575CD-95C4-EF47-857F-E77ADA073614}" name="ERASMUS CODE" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{E9FC6546-D578-6A42-A4DC-38DCFDCCDC46}" name="Město" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{ECC8EB01-6710-8747-9112-7A812A03367E}" name="Stát" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{322375E3-3C6A-3B4E-8975-3A19A72FE659}" name="Latitude" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{80E625A7-4E28-5D4C-A6F6-54153227E247}" name="Longtitude" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{6EE1A8B0-25EB-9345-82C2-79D3A3B62B2C}" name="URL" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{F1C2FD06-28A1-D847-971D-93220E657CA3}" name="Katedra" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{CDA11F7E-DE5E-5442-8805-D34B212F75F4}" name="Univerzita" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{27C575CD-95C4-EF47-857F-E77ADA073614}" name="ERASMUS CODE" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{E9FC6546-D578-6A42-A4DC-38DCFDCCDC46}" name="Město" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{ECC8EB01-6710-8747-9112-7A812A03367E}" name="Stát" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{322375E3-3C6A-3B4E-8975-3A19A72FE659}" name="Latitude" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{80E625A7-4E28-5D4C-A6F6-54153227E247}" name="Longtitude" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{6EE1A8B0-25EB-9345-82C2-79D3A3B62B2C}" name="URL" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1957,26 +1963,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6079A5C9-AB59-8A4D-94D1-942004316F7B}">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="38.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
-    <col min="8" max="8" width="38.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" customWidth="1"/>
-    <col min="11" max="11" width="38.1640625" customWidth="1"/>
+    <col min="2" max="2" width="38.19921875" customWidth="1"/>
+    <col min="3" max="3" width="27.19921875" customWidth="1"/>
+    <col min="4" max="4" width="18.19921875" customWidth="1"/>
+    <col min="5" max="5" width="28.296875" customWidth="1"/>
+    <col min="6" max="6" width="27.19921875" customWidth="1"/>
+    <col min="7" max="7" width="19.296875" customWidth="1"/>
+    <col min="8" max="8" width="38.796875" customWidth="1"/>
+    <col min="9" max="9" width="12.796875" customWidth="1"/>
+    <col min="11" max="11" width="38.19921875" customWidth="1"/>
     <col min="12" max="12" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2005,7 +2011,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="10"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -2034,7 +2040,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -2063,7 +2069,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>67</v>
       </c>
@@ -2092,7 +2098,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>67</v>
       </c>
@@ -2121,7 +2127,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>67</v>
       </c>
@@ -2150,7 +2156,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>80</v>
       </c>
@@ -2179,7 +2185,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>88</v>
       </c>
@@ -2208,7 +2214,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>134</v>
       </c>
@@ -2237,7 +2243,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>134</v>
       </c>
@@ -2266,7 +2272,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>141</v>
       </c>
@@ -2295,7 +2301,7 @@
       <c r="J11" s="5"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>141</v>
       </c>
@@ -2324,7 +2330,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>141</v>
       </c>
@@ -2353,7 +2359,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>141</v>
       </c>
@@ -2382,7 +2388,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>141</v>
       </c>
@@ -2411,7 +2417,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>88</v>
       </c>
@@ -2440,7 +2446,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>88</v>
       </c>
@@ -2469,7 +2475,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>141</v>
       </c>
@@ -2498,7 +2504,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>141</v>
       </c>
@@ -2527,7 +2533,7 @@
       <c r="J19" s="5"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>5</v>
       </c>
@@ -2556,7 +2562,7 @@
       <c r="J20" s="5"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>80</v>
       </c>
@@ -2585,7 +2591,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>88</v>
       </c>
@@ -2614,7 +2620,7 @@
       <c r="J22" s="5"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>134</v>
       </c>
@@ -2643,7 +2649,7 @@
       <c r="J23" s="6"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>141</v>
       </c>
@@ -2672,7 +2678,7 @@
       <c r="J24" s="6"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>5</v>
       </c>
@@ -2701,7 +2707,7 @@
       <c r="J25" s="6"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>5</v>
       </c>
@@ -2730,7 +2736,7 @@
       <c r="J26" s="6"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>67</v>
       </c>
@@ -2759,7 +2765,7 @@
       <c r="J27" s="6"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>80</v>
       </c>
@@ -2788,7 +2794,7 @@
       <c r="J28" s="6"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>80</v>
       </c>
@@ -2817,7 +2823,7 @@
       <c r="J29" s="6"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>88</v>
       </c>
@@ -2846,7 +2852,7 @@
       <c r="J30" s="6"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>88</v>
       </c>
@@ -2875,7 +2881,7 @@
       <c r="J31" s="6"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>88</v>
       </c>
@@ -2904,7 +2910,7 @@
       <c r="J32" s="6"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>88</v>
       </c>
@@ -2933,7 +2939,7 @@
       <c r="J33" s="6"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>88</v>
       </c>
@@ -2962,7 +2968,7 @@
       <c r="J34" s="6"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>88</v>
       </c>
@@ -2991,7 +2997,7 @@
       <c r="J35" s="6"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>88</v>
       </c>
@@ -3020,7 +3026,7 @@
       <c r="J36" s="6"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>134</v>
       </c>
@@ -3049,7 +3055,7 @@
       <c r="J37" s="6"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>141</v>
       </c>
@@ -3078,7 +3084,7 @@
       <c r="J38" s="6"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>141</v>
       </c>
@@ -3107,7 +3113,7 @@
       <c r="J39" s="6"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>141</v>
       </c>
@@ -3136,7 +3142,7 @@
       <c r="J40" s="6"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>141</v>
       </c>
@@ -3165,7 +3171,7 @@
       <c r="J41" s="6"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>5</v>
       </c>
@@ -3194,7 +3200,7 @@
       <c r="J42" s="6"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>141</v>
       </c>
@@ -3223,7 +3229,7 @@
       <c r="J43" s="6"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>5</v>
       </c>
@@ -3252,7 +3258,7 @@
       <c r="J44" s="6"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>5</v>
       </c>
@@ -3281,7 +3287,7 @@
       <c r="J45" s="6"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>67</v>
       </c>
@@ -3310,7 +3316,7 @@
       <c r="J46" s="6"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>67</v>
       </c>
@@ -3339,7 +3345,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>80</v>
       </c>
@@ -3366,7 +3372,7 @@
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>88</v>
       </c>
@@ -3393,7 +3399,7 @@
       </c>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>88</v>
       </c>
@@ -3420,7 +3426,7 @@
       </c>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>134</v>
       </c>
@@ -3447,7 +3453,7 @@
       </c>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>141</v>
       </c>
@@ -3474,7 +3480,7 @@
       </c>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>141</v>
       </c>
@@ -3500,7 +3506,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
         <v>88</v>
       </c>
@@ -3526,7 +3532,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>5</v>
       </c>
@@ -3552,7 +3558,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>5</v>
       </c>
@@ -3578,7 +3584,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>88</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>88</v>
       </c>
@@ -3630,7 +3636,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>141</v>
       </c>
@@ -3656,7 +3662,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
         <v>5</v>
       </c>
@@ -3682,7 +3688,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>67</v>
       </c>
@@ -3708,7 +3714,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
         <v>80</v>
       </c>
@@ -3734,7 +3740,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
         <v>88</v>
       </c>
@@ -3760,7 +3766,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>134</v>
       </c>
@@ -3786,7 +3792,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>141</v>
       </c>
@@ -3812,7 +3818,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
         <v>5</v>
       </c>
@@ -3838,7 +3844,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
         <v>5</v>
       </c>
@@ -3864,7 +3870,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>5</v>
       </c>
@@ -3890,7 +3896,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>67</v>
       </c>
@@ -3916,7 +3922,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
         <v>67</v>
       </c>
@@ -3942,7 +3948,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>88</v>
       </c>
@@ -3968,7 +3974,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
         <v>134</v>
       </c>
@@ -3994,7 +4000,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>134</v>
       </c>
@@ -4020,7 +4026,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
         <v>141</v>
       </c>
@@ -4046,7 +4052,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>141</v>
       </c>
@@ -4072,7 +4078,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
         <v>141</v>
       </c>
@@ -4098,7 +4104,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
         <v>141</v>
       </c>
@@ -4124,7 +4130,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
         <v>88</v>
       </c>
@@ -4150,7 +4156,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
         <v>88</v>
       </c>
@@ -4176,7 +4182,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
         <v>80</v>
       </c>
@@ -4202,7 +4208,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>134</v>
       </c>
@@ -4228,7 +4234,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
         <v>141</v>
       </c>
@@ -4254,7 +4260,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
         <v>141</v>
       </c>
@@ -4280,7 +4286,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
         <v>5</v>
       </c>
@@ -4306,7 +4312,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
         <v>5</v>
       </c>
@@ -4332,7 +4338,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
         <v>67</v>
       </c>
@@ -4358,7 +4364,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
         <v>80</v>
       </c>
@@ -4384,7 +4390,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
         <v>134</v>
       </c>
@@ -4410,7 +4416,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
         <v>141</v>
       </c>
@@ -4436,7 +4442,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
         <v>141</v>
       </c>
@@ -4462,7 +4468,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>141</v>
       </c>
@@ -4488,7 +4494,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
         <v>141</v>
       </c>
@@ -4514,7 +4520,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="8" t="s">
         <v>5</v>
       </c>
@@ -4540,7 +4546,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="s">
         <v>67</v>
       </c>
@@ -4566,7 +4572,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="11" t="s">
         <v>80</v>
       </c>

</xml_diff>